<commit_message>
refreash on post success,email validator and mail sent on certificate hash and saving
</commit_message>
<xml_diff>
--- a/BlockChain_code_File-main/public/excel/jt.xlsx
+++ b/BlockChain_code_File-main/public/excel/jt.xlsx
@@ -200,7 +200,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -255,6 +255,9 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -262,37 +265,7 @@
     <cellStyle name="Normal_TRUE" xfId="1"/>
     <cellStyle name="Normal_TRUE_2" xfId="2"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -472,19 +445,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:J5"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="S/No" dataDxfId="11"/>
-    <tableColumn id="2" name="Batch Code" dataDxfId="10" dataCellStyle="Normal_TRUE"/>
+    <tableColumn id="1" name="S/No" dataDxfId="8"/>
+    <tableColumn id="2" name="Batch Code" dataDxfId="7" dataCellStyle="Normal_TRUE"/>
     <tableColumn id="3" name="Staff_Name"/>
-    <tableColumn id="4" name="Staff_EmpNumber" dataDxfId="9"/>
-    <tableColumn id="5" name="TrainingTitle" dataDxfId="8"/>
-    <tableColumn id="6" name="TrainingCode" dataDxfId="7"/>
-    <tableColumn id="7" name="Batch_Trainer" dataDxfId="6"/>
-    <tableColumn id="8" name="BatchStartDate" dataDxfId="5" dataCellStyle="Normal_TRUE"/>
-    <tableColumn id="9" name="Staff_Email" dataDxfId="4" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" name="Certificate_Name" dataDxfId="3"/>
+    <tableColumn id="4" name="Staff_EmpNumber" dataDxfId="6"/>
+    <tableColumn id="5" name="TrainingTitle" dataDxfId="5"/>
+    <tableColumn id="6" name="TrainingCode" dataDxfId="4"/>
+    <tableColumn id="7" name="Batch_Trainer" dataDxfId="3"/>
+    <tableColumn id="8" name="BatchStartDate" dataDxfId="2" dataCellStyle="Normal_TRUE"/>
+    <tableColumn id="9" name="Staff_Email" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" name="Certificate_Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -745,7 +718,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -756,7 +729,7 @@
   <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -780,7 +753,7 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -2191,7 +2164,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D101">
-    <cfRule type="duplicateValues" dxfId="13" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
@@ -2205,61 +2178,61 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="RightsWATCHMark">76|Etisalat-Group-Internal|{00000000-0000-0000-0000-000000000000}</XMLData>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">10:19 01/09/2019</XMLData>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%HOSTNAME%">WCB00094282.etisalat.corp.ae</XMLData>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">10:19 01/09/2019</XMLData>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%USERNAME%">mohammshahin</XMLData>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="RightsWATCHMark">76|Etisalat-Group-Internal|{00000000-0000-0000-0000-000000000000}</XMLData>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%EMAILADDRESS%">mohammshahin@etisalat.ae</XMLData>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">mohammshahin</XMLData>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158E32D4-C0BA-4AEA-B8E7-E2B73F1D51AA}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5375092-E49A-46E6-A2BF-AF82C0840F59}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97F6B195-C060-43AA-A24A-6190B6CF0D70}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FD55538-6D4B-425F-B44D-4015B7E9E399}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97F6B195-C060-43AA-A24A-6190B6CF0D70}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5375092-E49A-46E6-A2BF-AF82C0840F59}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158E32D4-C0BA-4AEA-B8E7-E2B73F1D51AA}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF54BAE9-5F59-4D3F-ADAE-3F6AC2F1C876}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78B9DA3B-989B-4D15-9A99-8576DAF2B73D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78B9DA3B-989B-4D15-9A99-8576DAF2B73D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF54BAE9-5F59-4D3F-ADAE-3F6AC2F1C876}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>